<commit_message>
New version read.xlsx and incorp NA fix v3.4 ALFAM2
</commit_message>
<xml_diff>
--- a/inputs/inputs.xlsx
+++ b/inputs/inputs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Locations" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
     <sheet name="Settings" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="Units" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="Options" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="Vars (hidden)" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="Names" sheetId="8" state="visible" r:id="rId9"/>
     <sheet name="Directories" sheetId="9" state="visible" r:id="rId10"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -354,7 +354,7 @@
     <t xml:space="preserve">kg/t</t>
   </si>
   <si>
-    <t xml:space="preserve">Incorporation timing</t>
+    <t xml:space="preserve">Time</t>
   </si>
   <si>
     <t xml:space="preserve">Application methods</t>
@@ -1069,7 +1069,7 @@
   </sheetPr>
   <dimension ref="A1:O35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="K35" activeCellId="0" sqref="K35"/>
     </sheetView>
   </sheetViews>
@@ -2327,7 +2327,7 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2542,7 +2542,7 @@
   </sheetPr>
   <dimension ref="A1:O18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
blank template and example, more prep for sharing
</commit_message>
<xml_diff>
--- a/inputs/inputs.xlsx
+++ b/inputs/inputs.xlsx
@@ -5,20 +5,20 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Locations" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Slurry composition" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Application" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="Defaults" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="Settings" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="Units" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="Uncertainty" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="Settings" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Units" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Uncertainty" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="Defaults" sheetId="8" state="visible" r:id="rId9"/>
     <sheet name="Directories" sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="Names" sheetId="10" state="visible" r:id="rId11"/>
-    <sheet name="Options" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="Names" sheetId="10" state="hidden" r:id="rId11"/>
+    <sheet name="Options" sheetId="11" state="hidden" r:id="rId12"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="169">
   <si>
     <t xml:space="preserve">Combined input file for the ALFAMI R package for estimation of ammonia emission from field-applied slurry</t>
   </si>
@@ -83,19 +83,37 @@
     <t xml:space="preserve">Locations</t>
   </si>
   <si>
-    <t xml:space="preserve">Enter geographical location information, for linking application events to locations and aggregation variables through location key</t>
+    <t xml:space="preserve">Geographical location information, for linking application events to locations and aggregation variables through location key</t>
   </si>
   <si>
     <t xml:space="preserve">Slurry composition</t>
   </si>
   <si>
-    <t xml:space="preserve">Enter slurry composition for emission calculations (set in Defaults sheet if constant)</t>
+    <t xml:space="preserve">Slurry composition for emission calculations (set in Defaults sheet if constant)</t>
   </si>
   <si>
     <t xml:space="preserve">Application</t>
   </si>
   <si>
-    <t xml:space="preserve">Enter application events with details on location, slurry type, timing</t>
+    <t xml:space="preserve">Application events with details on location, slurry type, timing (the main worksheet)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Settings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Settings for uncertainty calculations and output file types</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Units</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set input and output units</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uncertainty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uncertainty inputs</t>
   </si>
   <si>
     <t xml:space="preserve">Defaults</t>
@@ -104,22 +122,10 @@
     <t xml:space="preserve">Optional: enter or check default inputs</t>
   </si>
   <si>
-    <t xml:space="preserve">Settings</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Settings for uncertainty calculations and output files</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Units</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Set input and output units</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Uncertainty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enter uncertainty inputs</t>
+    <t xml:space="preserve">Directories</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Optional: change directories for input, output, and logs</t>
   </si>
   <si>
     <t xml:space="preserve">Appearance key</t>
@@ -181,30 +187,6 @@
     <t xml:space="preserve">Aggregation group 2</t>
   </si>
   <si>
-    <t xml:space="preserve">North</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bigone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Smallone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Central</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Highone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">South</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Warmone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Otherone</t>
-  </si>
-  <si>
     <t xml:space="preserve">Slurry key</t>
   </si>
   <si>
@@ -220,30 +202,6 @@
     <t xml:space="preserve">pH</t>
   </si>
   <si>
-    <t xml:space="preserve">Cattle 2010s</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cattle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cattle 2020s</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pig 2010s</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pig</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pig 2020s</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pig special</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pig acidified 2020</t>
-  </si>
-  <si>
     <t xml:space="preserve">Application name</t>
   </si>
   <si>
@@ -292,358 +250,343 @@
     <t xml:space="preserve">D or DD (integer)</t>
   </si>
   <si>
-    <t xml:space="preserve">Cattle spring</t>
+    <t xml:space="preserve">Setting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parameter set</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALFAM2pars02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Include input uncertainty?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Include par uncertainty?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uncertainty iterations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uncertainty seed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Confidence level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weather type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Constant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Output digits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Output file name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Overwrite output?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type of output</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Variable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slurry mass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TAN mass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Land area</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t/ha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slurry dry matter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">% FM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">% of fresh mass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TAN concentration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kg/t</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Air temperature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">°C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wind speed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m/s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Input</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Absolute uncertainty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Relative uncertainty (frac.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lower limit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Upper limit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slurry pH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Default value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Application day of month</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Application time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HH:MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Emission duration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slurry TAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">File type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Directory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weather</t>
+  </si>
+  <si>
+    <t xml:space="preserve">weather</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Output</t>
+  </si>
+  <si>
+    <t xml:space="preserve">output</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Logs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">logs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weather locations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">loc.key</t>
+  </si>
+  <si>
+    <t xml:space="preserve">loc.agg1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">loc.agg2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">loc.name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">man.key</t>
+  </si>
+  <si>
+    <t xml:space="preserve">man.source</t>
+  </si>
+  <si>
+    <t xml:space="preserve">man.dm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">man.tan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">man.ph</t>
+  </si>
+  <si>
+    <t xml:space="preserve">app.key</t>
+  </si>
+  <si>
+    <t xml:space="preserve">app.year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">app.man</t>
+  </si>
+  <si>
+    <t xml:space="preserve">app.tan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">app.area</t>
+  </si>
+  <si>
+    <t xml:space="preserve">app.rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">app.mthd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">incorp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">incorp.time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wthr.year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wthr.month</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wthr.day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wthr.time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">emis.dur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">parset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uncert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">paruncert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">seedu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wthr.type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ndig</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ofile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">overwrite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">otype</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Application methods</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Incorporation options</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parameter sets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weather data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes/no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Output type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Broadcast</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shallow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALFAM2pars01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CSV</t>
   </si>
   <si>
     <t xml:space="preserve">Trailing hose</t>
   </si>
   <si>
-    <t xml:space="preserve">Cattle summer grass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Broadcast</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shallow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pig fall</t>
+    <t xml:space="preserve">Deep</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CSV2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trailing shoe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALFAM2pars03</t>
   </si>
   <si>
     <t xml:space="preserve">Open slot injection</t>
   </si>
   <si>
-    <t xml:space="preserve">Pig spring</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Input</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Default value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Application day of month</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Application time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HH:MM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">09:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Emission duration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Slurry dry matter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Slurry pH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Slurry TAN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Setting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parameter set</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ALFAM2pars02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Include input uncertainty?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Include par uncertainty?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Uncertainty iterations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Uncertainty seed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Confidence level</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Weather type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Constant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Output digits</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Output file name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Some_Country</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Overwrite output?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Type of output</t>
-  </si>
-  <si>
     <t xml:space="preserve">CSV and xlsx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Variable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Notes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Slurry mass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">t</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TAN mass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Land area</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ha</t>
-  </si>
-  <si>
-    <t xml:space="preserve">t/ha</t>
-  </si>
-  <si>
-    <t xml:space="preserve">% FM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">% of fresh mass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TAN concentration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kg/t</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Air temperature</t>
-  </si>
-  <si>
-    <t xml:space="preserve">°C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wind speed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">m/s</t>
-  </si>
-  <si>
-    <t xml:space="preserve">`</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Absolute uncertainty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Relative uncertainty (frac.)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lower limit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Upper limit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">File type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Directory</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Weather</t>
-  </si>
-  <si>
-    <t xml:space="preserve">weather</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Output</t>
-  </si>
-  <si>
-    <t xml:space="preserve">output</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Logs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">logs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Weather locations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">loc.key</t>
-  </si>
-  <si>
-    <t xml:space="preserve">loc.agg1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">loc.agg2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">loc.name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">man.key</t>
-  </si>
-  <si>
-    <t xml:space="preserve">man.source</t>
-  </si>
-  <si>
-    <t xml:space="preserve">man.dm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">man.tan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">man.ph</t>
-  </si>
-  <si>
-    <t xml:space="preserve">app.key</t>
-  </si>
-  <si>
-    <t xml:space="preserve">app.year</t>
-  </si>
-  <si>
-    <t xml:space="preserve">app.man</t>
-  </si>
-  <si>
-    <t xml:space="preserve">app.tan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">app.area</t>
-  </si>
-  <si>
-    <t xml:space="preserve">app.rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">app.mthd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">incorp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">incorp.time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wthr.year</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wthr.month</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wthr.day</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wthr.time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">emis.dur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">parset</t>
-  </si>
-  <si>
-    <t xml:space="preserve">uncert</t>
-  </si>
-  <si>
-    <t xml:space="preserve">paruncert</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">seedu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wthr.type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ndig</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ofile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">overwrite</t>
-  </si>
-  <si>
-    <t xml:space="preserve">otype</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Application methods</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Incorporation options</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parameter sets</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Weather data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes/no</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Output type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ALFAM2pars01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CSV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deep</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CSV2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trailing shoe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ALFAM2pars03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">xlsx</t>
   </si>
   <si>
     <t xml:space="preserve">Closed slot injection</t>
@@ -760,6 +703,12 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FF666666"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -771,12 +720,6 @@
       <color rgb="FF666666"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -1037,46 +980,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1089,6 +992,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1109,7 +1016,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1134,6 +1041,42 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1240,7 +1183,7 @@
   </sheetPr>
   <dimension ref="B2:D19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -1326,46 +1269,54 @@
         <v>17</v>
       </c>
     </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="7" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="8" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1417,7 +1368,7 @@
   <sheetData>
     <row r="1" s="58" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="57" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="B1" s="18"/>
       <c r="C1" s="18"/>
@@ -1452,16 +1403,16 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="56" t="s">
-        <v>138</v>
+        <v>116</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>139</v>
+        <v>117</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>140</v>
+        <v>118</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1503,19 +1454,19 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="56" t="s">
-        <v>142</v>
+        <v>120</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>143</v>
+        <v>121</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>145</v>
+        <v>123</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>146</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" s="58" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1597,46 +1548,46 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="56" t="s">
-        <v>147</v>
+        <v>125</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>138</v>
+        <v>116</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>148</v>
+        <v>126</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>142</v>
+        <v>120</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>149</v>
+        <v>127</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>150</v>
+        <v>128</v>
       </c>
       <c r="G11" s="18" t="s">
-        <v>151</v>
+        <v>129</v>
       </c>
       <c r="H11" s="18" t="s">
-        <v>152</v>
+        <v>130</v>
       </c>
       <c r="I11" s="18" t="s">
-        <v>153</v>
+        <v>131</v>
       </c>
       <c r="J11" s="18" t="s">
-        <v>154</v>
+        <v>132</v>
       </c>
       <c r="K11" s="18" t="s">
-        <v>155</v>
+        <v>133</v>
       </c>
       <c r="L11" s="18" t="s">
-        <v>156</v>
+        <v>134</v>
       </c>
       <c r="M11" s="18" t="s">
-        <v>157</v>
+        <v>135</v>
       </c>
       <c r="N11" s="18" t="s">
-        <v>158</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1644,7 +1595,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="57" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1653,7 +1604,7 @@
         <v>Application day of month</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>158</v>
+        <v>136</v>
       </c>
       <c r="C14" s="58"/>
       <c r="D14" s="58"/>
@@ -1664,7 +1615,7 @@
         <v>Application time</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>159</v>
+        <v>137</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1673,7 +1624,7 @@
         <v>Emission duration</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>160</v>
+        <v>138</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1682,7 +1633,7 @@
         <v>Application rate</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>152</v>
+        <v>130</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1690,7 +1641,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="57" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1699,7 +1650,7 @@
         <v>Parameter set</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>161</v>
+        <v>139</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1708,7 +1659,7 @@
         <v>Include input uncertainty?</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>162</v>
+        <v>140</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1717,7 +1668,7 @@
         <v>Include par uncertainty?</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>163</v>
+        <v>141</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1726,7 +1677,7 @@
         <v>Uncertainty iterations</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>164</v>
+        <v>142</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1735,7 +1686,7 @@
         <v>Uncertainty seed</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>165</v>
+        <v>143</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1744,7 +1695,7 @@
         <v>Confidence level</v>
       </c>
       <c r="B25" s="18" t="s">
-        <v>166</v>
+        <v>144</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1753,7 +1704,7 @@
         <v>Weather type</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>167</v>
+        <v>145</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1762,7 +1713,7 @@
         <v>Output digits</v>
       </c>
       <c r="B27" s="18" t="s">
-        <v>168</v>
+        <v>146</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1771,7 +1722,7 @@
         <v>Output file name</v>
       </c>
       <c r="B28" s="18" t="s">
-        <v>169</v>
+        <v>147</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1780,7 +1731,7 @@
         <v>Overwrite output?</v>
       </c>
       <c r="B29" s="18" t="s">
-        <v>170</v>
+        <v>148</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1789,7 +1740,7 @@
         <v>Type of output</v>
       </c>
       <c r="B30" s="18" t="s">
-        <v>171</v>
+        <v>149</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1797,7 +1748,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="57" t="s">
-        <v>133</v>
+        <v>111</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1858,7 +1809,7 @@
       <selection pane="topLeft" activeCell="K16" activeCellId="0" sqref="K16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.33"/>
@@ -1869,89 +1820,89 @@
   <sheetData>
     <row r="1" s="61" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="61" t="s">
-        <v>172</v>
+        <v>150</v>
       </c>
       <c r="C1" s="61" t="s">
-        <v>173</v>
+        <v>151</v>
       </c>
       <c r="E1" s="61" t="s">
-        <v>174</v>
+        <v>152</v>
       </c>
       <c r="G1" s="61" t="s">
-        <v>175</v>
+        <v>153</v>
       </c>
       <c r="I1" s="61" t="s">
-        <v>176</v>
+        <v>154</v>
       </c>
       <c r="K1" s="61" t="s">
-        <v>177</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>71</v>
+        <v>156</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>72</v>
+        <v>157</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>178</v>
+        <v>158</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>98</v>
+        <v>65</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>179</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>69</v>
+        <v>160</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>180</v>
+        <v>161</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>90</v>
+        <v>57</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>105</v>
+        <v>72</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>181</v>
+        <v>59</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>182</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>183</v>
+        <v>163</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>184</v>
+        <v>164</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>185</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>74</v>
+        <v>165</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>104</v>
+        <v>166</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>186</v>
+        <v>167</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>187</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -1970,10 +1921,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ6"/>
+  <dimension ref="A1:AMJ2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1988,13 +1939,13 @@
   <sheetData>
     <row r="1" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="13" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>3</v>
@@ -2007,60 +1958,10 @@
       <c r="AMJ1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="15" t="n">
-        <v>1000</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>31</v>
-      </c>
+      <c r="A2" s="15"/>
+      <c r="B2" s="16"/>
       <c r="C2" s="16"/>
-      <c r="D2" s="17" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9" t="n">
-        <v>1001</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="9" t="n">
-        <v>1002</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="9" t="n">
-        <v>1003</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="9" t="n">
-        <v>1004</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>38</v>
-      </c>
+      <c r="D2" s="17"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2081,7 +1982,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2096,19 +1997,19 @@
   <sheetData>
     <row r="1" s="14" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="13" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2123,106 +2024,14 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="C3" s="16" t="n">
-        <v>7</v>
-      </c>
-      <c r="D3" s="16" t="n">
-        <v>3</v>
-      </c>
-      <c r="E3" s="19" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="C4" s="18" t="n">
-        <v>6</v>
-      </c>
-      <c r="D4" s="18" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="E4" s="11" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="B5" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="C5" s="18" t="n">
-        <v>5</v>
-      </c>
-      <c r="D5" s="18" t="n">
-        <v>4</v>
-      </c>
-      <c r="E5" s="11" t="n">
-        <v>7.1</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="B6" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="C6" s="18" t="n">
-        <v>4</v>
-      </c>
-      <c r="D6" s="18" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="E6" s="11" t="n">
-        <v>7.1</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="B7" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="C7" s="18" t="n">
-        <v>3</v>
-      </c>
-      <c r="D7" s="18" t="n">
-        <v>4</v>
-      </c>
-      <c r="E7" s="11" t="n">
-        <v>7.4</v>
-      </c>
+      <c r="A3" s="15"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="19"/>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="B8" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="C8" s="18" t="n">
-        <v>3</v>
-      </c>
-      <c r="D8" s="18" t="n">
-        <v>4</v>
-      </c>
-      <c r="E8" s="20" t="n">
-        <v>6</v>
-      </c>
+      <c r="E8" s="20"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2247,7 +2056,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E11" activeCellId="0" sqref="E11"/>
+      <selection pane="bottomRight" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2272,62 +2081,62 @@
   <sheetData>
     <row r="1" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="14" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="I1" s="24" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="J1" s="24" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="K1" s="14" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="L1" s="14" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="M1" s="14" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="N1" s="14" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="AMI1" s="1"/>
       <c r="AMJ1" s="1"/>
     </row>
     <row r="2" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="14" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="E2" s="25" t="str">
         <f aca="false">Units!B2</f>
@@ -2346,386 +2155,131 @@
         <v>t/ha</v>
       </c>
       <c r="I2" s="24" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="J2" s="24" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="K2" s="14" t="str">
         <f aca="false">Units!B8</f>
         <v>kg/t</v>
       </c>
       <c r="L2" s="14" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="M2" s="14" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="N2" s="14" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="AMI2" s="1"/>
       <c r="AMJ2" s="1"/>
     </row>
     <row r="3" s="30" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="B3" s="26" t="n">
-        <v>1000</v>
-      </c>
-      <c r="C3" s="21" t="n">
-        <v>2019</v>
-      </c>
-      <c r="D3" s="26" t="s">
-        <v>44</v>
-      </c>
+      <c r="A3" s="21"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="26"/>
       <c r="E3" s="21"/>
-      <c r="F3" s="27" t="n">
-        <v>350</v>
-      </c>
+      <c r="F3" s="27"/>
       <c r="G3" s="21"/>
       <c r="H3" s="21"/>
-      <c r="I3" s="28" t="s">
-        <v>69</v>
-      </c>
+      <c r="I3" s="28"/>
       <c r="J3" s="28"/>
       <c r="K3" s="21"/>
-      <c r="L3" s="21" t="n">
-        <v>2019</v>
-      </c>
-      <c r="M3" s="21" t="n">
-        <v>4</v>
-      </c>
+      <c r="L3" s="21"/>
+      <c r="M3" s="21"/>
       <c r="N3" s="29"/>
       <c r="AMI3" s="1"/>
       <c r="AMJ3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="B4" s="22" t="n">
-        <v>1000</v>
-      </c>
-      <c r="C4" s="21" t="n">
-        <v>2019</v>
-      </c>
-      <c r="D4" s="26" t="s">
-        <v>44</v>
-      </c>
+      <c r="C4" s="21"/>
+      <c r="D4" s="26"/>
       <c r="E4" s="21"/>
-      <c r="F4" s="18" t="n">
-        <v>720</v>
-      </c>
-      <c r="I4" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="J4" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="K4" s="10" t="n">
-        <v>4</v>
-      </c>
-      <c r="L4" s="21" t="n">
-        <v>2019</v>
-      </c>
-      <c r="M4" s="18" t="n">
-        <v>6</v>
-      </c>
+      <c r="L4" s="21"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="B5" s="26" t="n">
-        <v>1000</v>
-      </c>
-      <c r="C5" s="21" t="n">
-        <v>2019</v>
-      </c>
-      <c r="D5" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="F5" s="18" t="n">
-        <v>1240</v>
-      </c>
+      <c r="B5" s="26"/>
+      <c r="C5" s="21"/>
       <c r="H5" s="27"/>
-      <c r="I5" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="L5" s="21" t="n">
-        <v>2019</v>
-      </c>
-      <c r="M5" s="18" t="n">
-        <v>9</v>
-      </c>
+      <c r="L5" s="21"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="B6" s="26" t="n">
-        <v>1001</v>
-      </c>
-      <c r="C6" s="21" t="n">
-        <v>2019</v>
-      </c>
-      <c r="D6" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="F6" s="18" t="n">
-        <v>3520</v>
-      </c>
-      <c r="I6" s="23" t="s">
-        <v>69</v>
-      </c>
-      <c r="L6" s="21" t="n">
-        <v>2019</v>
-      </c>
-      <c r="M6" s="18" t="n">
-        <v>5</v>
-      </c>
+      <c r="B6" s="26"/>
+      <c r="C6" s="21"/>
+      <c r="L6" s="21"/>
     </row>
     <row r="7" s="30" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="B7" s="26" t="n">
-        <v>1000</v>
-      </c>
-      <c r="C7" s="21" t="n">
-        <v>2020</v>
-      </c>
-      <c r="D7" s="26" t="s">
-        <v>46</v>
-      </c>
+      <c r="A7" s="21"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="26"/>
       <c r="E7" s="21"/>
-      <c r="F7" s="27" t="n">
-        <v>420</v>
-      </c>
+      <c r="F7" s="27"/>
       <c r="G7" s="21"/>
       <c r="H7" s="21"/>
-      <c r="I7" s="28" t="s">
-        <v>69</v>
-      </c>
+      <c r="I7" s="28"/>
       <c r="J7" s="28"/>
       <c r="K7" s="21"/>
-      <c r="L7" s="21" t="n">
-        <v>2020</v>
-      </c>
-      <c r="M7" s="21" t="n">
-        <v>4</v>
-      </c>
+      <c r="L7" s="21"/>
+      <c r="M7" s="21"/>
       <c r="N7" s="29"/>
       <c r="AMI7" s="1"/>
       <c r="AMJ7" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="B8" s="22" t="n">
-        <v>1000</v>
-      </c>
-      <c r="C8" s="21" t="n">
-        <v>2020</v>
-      </c>
-      <c r="D8" s="26" t="s">
-        <v>46</v>
-      </c>
+      <c r="C8" s="21"/>
+      <c r="D8" s="26"/>
       <c r="E8" s="21"/>
-      <c r="F8" s="18" t="n">
-        <v>1000</v>
-      </c>
-      <c r="I8" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="J8" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="K8" s="10" t="n">
-        <v>2</v>
-      </c>
-      <c r="L8" s="21" t="n">
-        <v>2020</v>
-      </c>
-      <c r="M8" s="18" t="n">
-        <v>6</v>
-      </c>
+      <c r="L8" s="21"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="B9" s="26" t="n">
-        <v>1000</v>
-      </c>
-      <c r="C9" s="21" t="n">
-        <v>2020</v>
-      </c>
-      <c r="D9" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="F9" s="18" t="n">
-        <v>1190</v>
-      </c>
+      <c r="B9" s="26"/>
+      <c r="C9" s="21"/>
       <c r="H9" s="27"/>
-      <c r="I9" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="L9" s="21" t="n">
-        <v>2020</v>
-      </c>
-      <c r="M9" s="18" t="n">
-        <v>9</v>
-      </c>
+      <c r="L9" s="21"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="B10" s="26" t="n">
-        <v>1001</v>
-      </c>
-      <c r="C10" s="21" t="n">
-        <v>2020</v>
-      </c>
-      <c r="D10" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="F10" s="18" t="n">
-        <v>3300</v>
-      </c>
-      <c r="I10" s="23" t="s">
-        <v>69</v>
-      </c>
-      <c r="L10" s="21" t="n">
-        <v>2020</v>
-      </c>
-      <c r="M10" s="18" t="n">
-        <v>5</v>
-      </c>
+      <c r="B10" s="26"/>
+      <c r="C10" s="21"/>
+      <c r="L10" s="21"/>
     </row>
     <row r="11" s="30" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="B11" s="26" t="n">
-        <v>1000</v>
-      </c>
-      <c r="C11" s="21" t="n">
-        <v>2021</v>
-      </c>
-      <c r="D11" s="26" t="s">
-        <v>44</v>
-      </c>
+      <c r="A11" s="21"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="26"/>
       <c r="E11" s="21"/>
-      <c r="F11" s="27" t="n">
-        <v>350</v>
-      </c>
+      <c r="F11" s="27"/>
       <c r="G11" s="21"/>
       <c r="H11" s="21"/>
-      <c r="I11" s="28" t="s">
-        <v>69</v>
-      </c>
+      <c r="I11" s="28"/>
       <c r="J11" s="28"/>
       <c r="K11" s="21"/>
-      <c r="L11" s="21" t="n">
-        <v>2019</v>
-      </c>
-      <c r="M11" s="21" t="n">
-        <v>4</v>
-      </c>
+      <c r="L11" s="21"/>
+      <c r="M11" s="21"/>
       <c r="N11" s="29"/>
       <c r="AMI11" s="1"/>
       <c r="AMJ11" s="1"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="B12" s="22" t="n">
-        <v>1000</v>
-      </c>
-      <c r="C12" s="21" t="n">
-        <v>2021</v>
-      </c>
-      <c r="D12" s="26" t="s">
-        <v>44</v>
-      </c>
+      <c r="C12" s="21"/>
+      <c r="D12" s="26"/>
       <c r="E12" s="21"/>
-      <c r="F12" s="18" t="n">
-        <v>720</v>
-      </c>
-      <c r="I12" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="J12" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="K12" s="10" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="L12" s="21" t="n">
-        <v>2019</v>
-      </c>
-      <c r="M12" s="18" t="n">
-        <v>6</v>
-      </c>
+      <c r="L12" s="21"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="B13" s="26" t="n">
-        <v>1000</v>
-      </c>
-      <c r="C13" s="21" t="n">
-        <v>2021</v>
-      </c>
-      <c r="D13" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="F13" s="18" t="n">
-        <v>1240</v>
-      </c>
+      <c r="B13" s="26"/>
+      <c r="C13" s="21"/>
       <c r="H13" s="27"/>
-      <c r="I13" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="L13" s="21" t="n">
-        <v>2019</v>
-      </c>
-      <c r="M13" s="18" t="n">
-        <v>9</v>
-      </c>
+      <c r="L13" s="21"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="B14" s="26" t="n">
-        <v>1001</v>
-      </c>
-      <c r="C14" s="21" t="n">
-        <v>2021</v>
-      </c>
-      <c r="D14" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="F14" s="18" t="n">
-        <v>3520</v>
-      </c>
-      <c r="I14" s="23" t="s">
-        <v>69</v>
-      </c>
-      <c r="L14" s="21" t="n">
-        <v>2019</v>
-      </c>
-      <c r="M14" s="18" t="n">
-        <v>5</v>
-      </c>
+      <c r="B14" s="26"/>
+      <c r="C14" s="21"/>
+      <c r="L14" s="21"/>
     </row>
     <row r="15" s="30" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="21"/>
@@ -2926,7 +2480,7 @@
       <formula1>Options!$C$2:$C$5</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E1:E1010" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E1:E1002" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -2947,152 +2501,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="12" width="25.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="12" width="23.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="12" width="17.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="31" width="12.68"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="5" style="12" width="11.57"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="D1" s="32" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="33" t="s">
-        <v>79</v>
-      </c>
-      <c r="B2" s="33" t="s">
-        <v>67</v>
-      </c>
-      <c r="C2" s="34"/>
-      <c r="D2" s="31" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="35" t="s">
-        <v>80</v>
-      </c>
-      <c r="B3" s="35" t="s">
-        <v>81</v>
-      </c>
-      <c r="C3" s="36"/>
-      <c r="D3" s="37" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="35" t="s">
-        <v>83</v>
-      </c>
-      <c r="B4" s="25" t="str">
-        <f aca="false">Units!B8</f>
-        <v>kg/t</v>
-      </c>
-      <c r="C4" s="38"/>
-      <c r="D4" s="31" t="n">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="B5" s="25" t="str">
-        <f aca="false">Units!B5</f>
-        <v>t/ha</v>
-      </c>
-      <c r="C5" s="38" t="n">
-        <v>30</v>
-      </c>
-      <c r="D5" s="31" t="n">
-        <v>40</v>
-      </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="B6" s="25" t="str">
-        <f aca="false">Units!B6</f>
-        <v>% FM</v>
-      </c>
-      <c r="C6" s="39"/>
-      <c r="D6" s="31" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="B7" s="25"/>
-      <c r="C7" s="38"/>
-      <c r="D7" s="31" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="B8" s="25" t="str">
-        <f aca="false">Units!B7</f>
-        <v>kg/t</v>
-      </c>
-      <c r="C8" s="40"/>
-      <c r="D8" s="31" t="n">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C6" type="list">
-      <formula1>Options!$G$2:$G$3</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-  </dataValidations>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:B12"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3104,98 +2516,90 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
-        <v>87</v>
+        <v>54</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>88</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="41" t="s">
-        <v>89</v>
-      </c>
-      <c r="B2" s="42" t="s">
-        <v>90</v>
+      <c r="A2" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B3" s="43" t="s">
-        <v>92</v>
+        <v>58</v>
+      </c>
+      <c r="B3" s="33" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B4" s="43" t="s">
-        <v>92</v>
+        <v>60</v>
+      </c>
+      <c r="B4" s="33" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B5" s="38" t="n">
-        <v>100</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="B5" s="34"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B6" s="38" t="n">
-        <v>1201</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="B6" s="34"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B7" s="38" t="n">
-        <v>0.75</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="B7" s="34"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B8" s="43" t="s">
-        <v>98</v>
+        <v>64</v>
+      </c>
+      <c r="B8" s="33" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B9" s="38" t="n">
+        <v>66</v>
+      </c>
+      <c r="B9" s="34" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B10" s="38" t="s">
-        <v>101</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="B10" s="34"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="B11" s="43" t="s">
-        <v>92</v>
+        <v>68</v>
+      </c>
+      <c r="B11" s="33" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B12" s="44" t="s">
-        <v>104</v>
+        <v>70</v>
+      </c>
+      <c r="B12" s="35" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -3227,7 +2631,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -3248,102 +2652,250 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
-        <v>105</v>
+        <v>72</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>106</v>
+        <v>73</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>107</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="B2" s="45" t="s">
-        <v>109</v>
-      </c>
-      <c r="C2" s="46"/>
+        <v>75</v>
+      </c>
+      <c r="B2" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="37"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="B3" s="47" t="s">
-        <v>109</v>
-      </c>
-      <c r="C3" s="48"/>
+        <v>77</v>
+      </c>
+      <c r="B3" s="38" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" s="39"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B4" s="47" t="s">
-        <v>112</v>
-      </c>
-      <c r="C4" s="48"/>
+        <v>78</v>
+      </c>
+      <c r="B4" s="38" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" s="39"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B5" s="47" t="s">
-        <v>113</v>
-      </c>
-      <c r="C5" s="48"/>
+        <v>43</v>
+      </c>
+      <c r="B5" s="38" t="s">
+        <v>80</v>
+      </c>
+      <c r="C5" s="39"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B6" s="47" t="s">
-        <v>114</v>
-      </c>
-      <c r="C6" s="48" t="s">
-        <v>115</v>
+        <v>81</v>
+      </c>
+      <c r="B6" s="38" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" s="39" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B7" s="47" t="s">
-        <v>117</v>
-      </c>
-      <c r="C7" s="48"/>
+        <v>84</v>
+      </c>
+      <c r="B7" s="38" t="s">
+        <v>85</v>
+      </c>
+      <c r="C7" s="39"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B8" s="47" t="s">
-        <v>117</v>
-      </c>
-      <c r="C8" s="48"/>
+        <v>86</v>
+      </c>
+      <c r="B8" s="38" t="s">
+        <v>85</v>
+      </c>
+      <c r="C8" s="39"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B9" s="49" t="s">
-        <v>120</v>
-      </c>
-      <c r="C9" s="48"/>
+        <v>87</v>
+      </c>
+      <c r="B9" s="40" t="s">
+        <v>88</v>
+      </c>
+      <c r="C9" s="39"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="B10" s="50" t="s">
-        <v>122</v>
-      </c>
-      <c r="C10" s="51"/>
+        <v>89</v>
+      </c>
+      <c r="B10" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="C10" s="42"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E20" s="1" t="s">
-        <v>123</v>
-      </c>
+        <v>91</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="12" width="23.94"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="5" style="12" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="1" width="11.57"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="7" t="str">
+        <f aca="false">Units!B6</f>
+        <v>% FM</v>
+      </c>
+      <c r="C2" s="43"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="37"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3" s="44"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="39"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="25" t="str">
+        <f aca="false">Units!B5</f>
+        <v>t/ha</v>
+      </c>
+      <c r="C4" s="44"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="39"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="25" t="str">
+        <f aca="false">Units!B2</f>
+        <v>t</v>
+      </c>
+      <c r="C5" s="44"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="39"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="25" t="str">
+        <f aca="false">Units!B8</f>
+        <v>kg/t</v>
+      </c>
+      <c r="C6" s="44"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="39"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B7" s="25" t="str">
+        <f aca="false">Units!B9</f>
+        <v>°C</v>
+      </c>
+      <c r="C7" s="44"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="39"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B8" s="25" t="str">
+        <f aca="false">Units!B10</f>
+        <v>m/s</v>
+      </c>
+      <c r="C8" s="45"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="42"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3364,150 +2916,128 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="12" width="23.94"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="5" style="12" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="1" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="12" width="25.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="12" width="23.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="12" width="17.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="47" width="12.68"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="5" style="12" width="11.57"/>
   </cols>
   <sheetData>
-    <row r="1" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="14" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>126</v>
-      </c>
-      <c r="F1" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>128</v>
+        <v>99</v>
+      </c>
+      <c r="D1" s="48" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B2" s="7" t="str">
+      <c r="A2" s="49" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2" s="49" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="50"/>
+      <c r="D2" s="47" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="51" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3" s="51" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3" s="52"/>
+      <c r="D3" s="53" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="51" t="s">
+        <v>105</v>
+      </c>
+      <c r="B4" s="25" t="str">
+        <f aca="false">Units!B8</f>
+        <v>kg/t</v>
+      </c>
+      <c r="C4" s="34"/>
+      <c r="D4" s="47" t="n">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="25" t="str">
+        <f aca="false">Units!B5</f>
+        <v>t/ha</v>
+      </c>
+      <c r="C5" s="34"/>
+      <c r="D5" s="47" t="n">
+        <v>40</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6" s="25" t="str">
         <f aca="false">Units!B6</f>
         <v>% FM</v>
       </c>
-      <c r="C2" s="52" t="n">
-        <v>2</v>
-      </c>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="46"/>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C3" s="53" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="48"/>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B4" s="25" t="str">
-        <f aca="false">Units!B5</f>
-        <v>t/ha</v>
-      </c>
-      <c r="C4" s="53"/>
-      <c r="D4" s="18" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="48"/>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B5" s="25" t="str">
-        <f aca="false">Units!B2</f>
-        <v>t</v>
-      </c>
-      <c r="C5" s="53"/>
-      <c r="D5" s="18" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="48"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B6" s="25" t="str">
-        <f aca="false">Units!B8</f>
+      <c r="C6" s="54"/>
+      <c r="D6" s="47" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" s="25"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="47" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="B8" s="25" t="str">
+        <f aca="false">Units!B7</f>
         <v>kg/t</v>
       </c>
-      <c r="C6" s="53" t="n">
-        <v>2</v>
-      </c>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="48"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B7" s="25" t="str">
-        <f aca="false">Units!B9</f>
-        <v>°C</v>
-      </c>
-      <c r="C7" s="53" t="n">
-        <v>2</v>
-      </c>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="48"/>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="B8" s="25" t="str">
-        <f aca="false">Units!B10</f>
-        <v>m/s</v>
-      </c>
-      <c r="C8" s="54" t="n">
-        <v>1</v>
-      </c>
-      <c r="D8" s="55"/>
-      <c r="E8" s="55"/>
-      <c r="F8" s="55"/>
-      <c r="G8" s="51"/>
+      <c r="C8" s="55"/>
+      <c r="D8" s="47" t="n">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C6" type="list">
+      <formula1>Options!$G$2:$G$3</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -3537,34 +3067,34 @@
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
-        <v>129</v>
+        <v>107</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>130</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="45" t="s">
-        <v>131</v>
-      </c>
-      <c r="B2" s="46" t="s">
-        <v>132</v>
+      <c r="A2" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" s="37" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="47" t="s">
-        <v>133</v>
-      </c>
-      <c r="B3" s="48" t="s">
-        <v>134</v>
+      <c r="A3" s="38" t="s">
+        <v>111</v>
+      </c>
+      <c r="B3" s="39" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="50" t="s">
-        <v>135</v>
-      </c>
-      <c r="B4" s="51" t="s">
-        <v>136</v>
+      <c r="A4" s="41" t="s">
+        <v>113</v>
+      </c>
+      <c r="B4" s="42" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Move uncert dist stuff to separate func.
And improve/expand uncert calcs with centered min/max.
Works with inputs.xlsx, still have not updated template.xlsx
</commit_message>
<xml_diff>
--- a/inputs/inputs.xlsx
+++ b/inputs/inputs.xlsx
@@ -66,8 +66,83 @@
 </comments>
 </file>
 
+<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author>SDH</author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Relative uncertainty means unit is fraction, e.g., -0.2 = 20% below normal input value.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">For normal distribution</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">For uniform, PERT, and triangular distribution. Takes mode from other inputs.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">For uniform, PERT, and triangular distributions. Mode taken as 0, and resulting uncertainty added to other inputs.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">For PERT</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="218">
   <si>
     <t xml:space="preserve">Combined input file for the ALFAMI R package for estimation of ammonia emission from field-applied slurry</t>
   </si>
@@ -443,231 +518,261 @@
     <t xml:space="preserve">m/s</t>
   </si>
   <si>
+    <t xml:space="preserve">(Any)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frac. input value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For relative uncertainty</t>
+  </si>
+  <si>
     <t xml:space="preserve">`</t>
   </si>
   <si>
     <t xml:space="preserve">Input</t>
   </si>
   <si>
+    <t xml:space="preserve">Uncertainty type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Distribution type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Standard deviation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minimum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maximum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Centered minimum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Centered maximum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shape</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Absolute</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PERT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slurry pH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Triangular</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Relative</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uniform</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Normal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Default value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Source</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Application day of month</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assumed, middle of month</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Application time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HH:MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assumed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average from ALFAM2 database vx.x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slurry TAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parameter set</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALFAM2pars03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uncertainty seed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Emission duration (h)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">File type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Directory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weather</t>
+  </si>
+  <si>
+    <t xml:space="preserve">weather</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Output</t>
+  </si>
+  <si>
+    <t xml:space="preserve">output</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Logs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">logs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weather locations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">loc.key</t>
+  </si>
+  <si>
+    <t xml:space="preserve">loc.agg1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">loc.agg2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">loc.name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">man.key</t>
+  </si>
+  <si>
+    <t xml:space="preserve">man.source</t>
+  </si>
+  <si>
+    <t xml:space="preserve">man.dm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">man.tan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">man.ph</t>
+  </si>
+  <si>
+    <t xml:space="preserve">app.key</t>
+  </si>
+  <si>
+    <t xml:space="preserve">app.year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">app.man</t>
+  </si>
+  <si>
+    <t xml:space="preserve">app.tan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">app.area</t>
+  </si>
+  <si>
+    <t xml:space="preserve">app.rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">app.mthd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">incorp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">incorp.time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wthr.year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wthr.month</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wthr.day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wthr.time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uncert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">paruncert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wthr.type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ndig</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ofile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">overwrite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">otype</t>
+  </si>
+  <si>
+    <t xml:space="preserve">parset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">seedu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">emis.dur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Application methods</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Incorporation options</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parameter sets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weather data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes/no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Output type</t>
+  </si>
+  <si>
     <t xml:space="preserve">Relative or absolute</t>
   </si>
   <si>
-    <t xml:space="preserve">Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Standard deviation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Minimum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maximum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shape</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Slurry pH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Absolute</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Normal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Default value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Source</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Application day of month</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Assumed, middle of month</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Application time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HH:MM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">09:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Assumed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Average from ALFAM2 database vx.x</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Slurry TAN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parameter set</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ALFAM2pars03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Uncertainty seed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Emission duration (h)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">File type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Directory</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Weather</t>
-  </si>
-  <si>
-    <t xml:space="preserve">weather</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Output</t>
-  </si>
-  <si>
-    <t xml:space="preserve">output</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Logs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">logs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Weather locations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">loc.key</t>
-  </si>
-  <si>
-    <t xml:space="preserve">loc.agg1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">loc.agg2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">loc.name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">man.key</t>
-  </si>
-  <si>
-    <t xml:space="preserve">man.source</t>
-  </si>
-  <si>
-    <t xml:space="preserve">man.dm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">man.tan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">man.ph</t>
-  </si>
-  <si>
-    <t xml:space="preserve">app.key</t>
-  </si>
-  <si>
-    <t xml:space="preserve">app.year</t>
-  </si>
-  <si>
-    <t xml:space="preserve">app.man</t>
-  </si>
-  <si>
-    <t xml:space="preserve">app.tan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">app.area</t>
-  </si>
-  <si>
-    <t xml:space="preserve">app.rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">app.mthd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">incorp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">incorp.time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wthr.year</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wthr.month</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wthr.day</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wthr.time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">uncert</t>
-  </si>
-  <si>
-    <t xml:space="preserve">paruncert</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wthr.type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ndig</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ofile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">overwrite</t>
-  </si>
-  <si>
-    <t xml:space="preserve">otype</t>
-  </si>
-  <si>
-    <t xml:space="preserve">parset</t>
-  </si>
-  <si>
-    <t xml:space="preserve">seedu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">emis.dur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Application methods</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Incorporation options</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parameter sets</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Weather data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes/no</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Output type</t>
-  </si>
-  <si>
     <t xml:space="preserve">Mean or mode</t>
   </si>
   <si>
@@ -677,9 +782,6 @@
     <t xml:space="preserve">ALFAM2pars01</t>
   </si>
   <si>
-    <t xml:space="preserve">Relative</t>
-  </si>
-  <si>
     <t xml:space="preserve">Mean (average)</t>
   </si>
   <si>
@@ -698,9 +800,6 @@
     <t xml:space="preserve">Mode (most likely)</t>
   </si>
   <si>
-    <t xml:space="preserve">Uniform</t>
-  </si>
-  <si>
     <t xml:space="preserve">Trailing shoe</t>
   </si>
   <si>
@@ -710,13 +809,7 @@
     <t xml:space="preserve">xlsx</t>
   </si>
   <si>
-    <t xml:space="preserve">PERT</t>
-  </si>
-  <si>
     <t xml:space="preserve">CSV and xlsx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Triangular</t>
   </si>
   <si>
     <t xml:space="preserve">Closed slot injection</t>
@@ -992,7 +1085,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="61">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1129,36 +1222,44 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -1315,7 +1416,7 @@
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="1.71"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="4" style="1" width="11.57"/>
   </cols>
@@ -1496,34 +1597,34 @@
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="28" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="30" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
       <c r="B3" s="31" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="33" t="s">
-        <v>150</v>
+        <v>159</v>
       </c>
       <c r="B4" s="34" t="s">
-        <v>151</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -1550,8 +1651,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="53" width="26.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="11" width="19.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="55" width="26.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="11" width="19.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="11" width="11.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="11" width="17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="11" width="15.15"/>
@@ -1561,59 +1662,59 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="11" width="13.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="11" width="18.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="11" width="12.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="11" width="17.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="11" width="17.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="11" width="15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="11" width="15.71"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="16" style="11" width="11.57"/>
   </cols>
   <sheetData>
-    <row r="1" s="55" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="54" t="s">
-        <v>152</v>
+    <row r="1" s="57" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="56" t="s">
+        <v>161</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
       <c r="D1" s="11"/>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="56" t="str">
+      <c r="A2" s="58" t="str">
         <f aca="false">Locations!A1</f>
         <v>Location key</v>
       </c>
-      <c r="B2" s="55" t="str">
+      <c r="B2" s="57" t="str">
         <f aca="false">Locations!B1</f>
         <v>Aggregation group 1</v>
       </c>
-      <c r="C2" s="55" t="str">
+      <c r="C2" s="57" t="str">
         <f aca="false">Locations!C1</f>
         <v>Aggregation group 2</v>
       </c>
-      <c r="D2" s="55" t="str">
+      <c r="D2" s="57" t="str">
         <f aca="false">Locations!D1</f>
         <v>Description</v>
       </c>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="53" t="s">
-        <v>153</v>
+      <c r="A3" s="55" t="s">
+        <v>162</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>155</v>
+        <v>164</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="5" s="55" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="54" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="5" s="57" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="56" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="11"/>
@@ -1621,46 +1722,46 @@
       <c r="D5" s="11"/>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="56" t="str">
+      <c r="A6" s="58" t="str">
         <f aca="false">'Slurry composition'!A1</f>
         <v>Slurry key</v>
       </c>
-      <c r="B6" s="55" t="str">
+      <c r="B6" s="57" t="str">
         <f aca="false">'Slurry composition'!B1</f>
         <v>Animal</v>
       </c>
-      <c r="C6" s="55" t="str">
+      <c r="C6" s="57" t="str">
         <f aca="false">'Slurry composition'!C1</f>
         <v>Dry matter</v>
       </c>
-      <c r="D6" s="55" t="str">
+      <c r="D6" s="57" t="str">
         <f aca="false">'Slurry composition'!D1</f>
         <v>TAN</v>
       </c>
-      <c r="E6" s="55" t="str">
+      <c r="E6" s="57" t="str">
         <f aca="false">'Slurry composition'!E1</f>
         <v>pH</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="53" t="s">
-        <v>157</v>
+      <c r="A7" s="55" t="s">
+        <v>166</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>159</v>
+        <v>168</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>160</v>
+        <v>169</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="9" s="55" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="54" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="9" s="57" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="56" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="11"/>
@@ -1668,319 +1769,319 @@
       <c r="D9" s="11"/>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="56" t="str">
+      <c r="A10" s="58" t="str">
         <f aca="false">Application!A1</f>
         <v>Application event name</v>
       </c>
-      <c r="B10" s="55" t="str">
+      <c r="B10" s="57" t="str">
         <f aca="false">Application!B1</f>
         <v>Location key</v>
       </c>
-      <c r="C10" s="55" t="str">
+      <c r="C10" s="57" t="str">
         <f aca="false">Application!C1</f>
         <v>Application year</v>
       </c>
-      <c r="D10" s="55" t="str">
+      <c r="D10" s="57" t="str">
         <f aca="false">Application!D1</f>
         <v>Slurry key</v>
       </c>
-      <c r="E10" s="55" t="str">
+      <c r="E10" s="57" t="str">
         <f aca="false">Application!E1</f>
         <v>Slurry application</v>
       </c>
-      <c r="F10" s="55" t="str">
+      <c r="F10" s="57" t="str">
         <f aca="false">Application!F1</f>
         <v>TAN application</v>
       </c>
-      <c r="G10" s="55" t="str">
+      <c r="G10" s="57" t="str">
         <f aca="false">Application!G1</f>
         <v>Application area</v>
       </c>
-      <c r="H10" s="55" t="str">
+      <c r="H10" s="57" t="str">
         <f aca="false">Application!H1</f>
         <v>Application rate</v>
       </c>
-      <c r="I10" s="55" t="str">
+      <c r="I10" s="57" t="str">
         <f aca="false">Application!I1</f>
         <v>Application method</v>
       </c>
-      <c r="J10" s="55" t="str">
+      <c r="J10" s="57" t="str">
         <f aca="false">Application!J1</f>
         <v>Incorporation</v>
       </c>
-      <c r="K10" s="55" t="str">
+      <c r="K10" s="57" t="str">
         <f aca="false">Application!K1</f>
         <v>Incorporation delay</v>
       </c>
-      <c r="L10" s="55" t="str">
+      <c r="L10" s="57" t="str">
         <f aca="false">Application!L1</f>
         <v>Weather year</v>
       </c>
-      <c r="M10" s="55" t="str">
+      <c r="M10" s="57" t="str">
         <f aca="false">Application!M1</f>
         <v>Application month</v>
       </c>
-      <c r="N10" s="55" t="str">
+      <c r="N10" s="57" t="str">
         <f aca="false">Application!N1</f>
         <v>Application day</v>
       </c>
-      <c r="O10" s="55"/>
+      <c r="O10" s="57"/>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="53" t="s">
+      <c r="A11" s="55" t="s">
+        <v>171</v>
+      </c>
+      <c r="B11" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="B11" s="11" t="s">
-        <v>153</v>
-      </c>
       <c r="C11" s="11" t="s">
-        <v>163</v>
+        <v>172</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>165</v>
+        <v>174</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>166</v>
+        <v>175</v>
       </c>
       <c r="H11" s="11" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="I11" s="11" t="s">
-        <v>168</v>
+        <v>177</v>
       </c>
       <c r="J11" s="11" t="s">
-        <v>169</v>
+        <v>178</v>
       </c>
       <c r="K11" s="11" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="L11" s="11" t="s">
-        <v>171</v>
+        <v>180</v>
       </c>
       <c r="M11" s="11" t="s">
-        <v>172</v>
+        <v>181</v>
       </c>
       <c r="N11" s="11" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="54" t="s">
+      <c r="A13" s="56" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="56" t="str">
+      <c r="A14" s="58" t="str">
         <f aca="false">Defaults!A2</f>
         <v>Application day of month</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>173</v>
-      </c>
-      <c r="C14" s="55"/>
-      <c r="D14" s="55"/>
+        <v>182</v>
+      </c>
+      <c r="C14" s="57"/>
+      <c r="D14" s="57"/>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="57" t="str">
+      <c r="A15" s="59" t="str">
         <f aca="false">Defaults!A3</f>
         <v>Application time</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="56" t="str">
+      <c r="A16" s="58" t="str">
         <f aca="false">Defaults!A4</f>
         <v>Application rate</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="56" t="str">
+      <c r="A17" s="58" t="str">
         <f aca="false">Defaults!A5</f>
         <v>Slurry dry matter</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>159</v>
+        <v>168</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="56" t="str">
+      <c r="A18" s="58" t="str">
         <f aca="false">Defaults!A6</f>
         <v>Slurry pH</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="56" t="str">
+      <c r="A19" s="58" t="str">
         <f aca="false">Defaults!A7</f>
         <v>Slurry TAN</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>160</v>
+        <v>169</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="56"/>
+      <c r="A20" s="58"/>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="54" t="s">
+      <c r="A21" s="56" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="56" t="str">
+      <c r="A22" s="58" t="str">
         <f aca="false">Settings!A2</f>
         <v>Include input uncertainty?</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>175</v>
+        <v>184</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="56" t="str">
+      <c r="A23" s="58" t="str">
         <f aca="false">Settings!A3</f>
         <v>Include par uncertainty?</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>176</v>
+        <v>185</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="56" t="str">
+      <c r="A24" s="58" t="str">
         <f aca="false">Settings!A4</f>
         <v>Uncertainty iterations</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>177</v>
+        <v>186</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="56" t="str">
+      <c r="A25" s="58" t="str">
         <f aca="false">Settings!A5</f>
         <v>Confidence level</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>178</v>
+        <v>187</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="56" t="str">
+      <c r="A26" s="58" t="str">
         <f aca="false">Settings!A6</f>
         <v>Weather resolution</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>179</v>
+        <v>188</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="56" t="str">
+      <c r="A27" s="58" t="str">
         <f aca="false">Settings!A7</f>
         <v>Output digits</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>180</v>
+        <v>189</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="56" t="str">
+      <c r="A28" s="58" t="str">
         <f aca="false">Settings!A8</f>
         <v>Output file name</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>181</v>
+        <v>190</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="56" t="str">
+      <c r="A29" s="58" t="str">
         <f aca="false">Settings!A9</f>
         <v>Overwrite output?</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>182</v>
+        <v>191</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="56" t="str">
+      <c r="A30" s="58" t="str">
         <f aca="false">Settings!A10</f>
         <v>Type of output</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>183</v>
+        <v>192</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="56"/>
+      <c r="A31" s="58"/>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="54" t="s">
+      <c r="A32" s="56" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="56" t="str">
+      <c r="A33" s="58" t="str">
         <f aca="false">Reproducibility!A2</f>
         <v>Parameter set</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>184</v>
+        <v>193</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="56" t="str">
+      <c r="A34" s="58" t="str">
         <f aca="false">Reproducibility!A3</f>
         <v>Uncertainty seed</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>185</v>
+        <v>194</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="56" t="str">
+      <c r="A35" s="58" t="str">
         <f aca="false">Reproducibility!A4</f>
         <v>Emission duration (h)</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>186</v>
+        <v>195</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="56"/>
+      <c r="A36" s="58"/>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="56"/>
+      <c r="A37" s="58"/>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="56"/>
+      <c r="A38" s="58"/>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="56"/>
+      <c r="A39" s="58"/>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="56"/>
+      <c r="A40" s="58"/>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="56"/>
+      <c r="A41" s="58"/>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="56"/>
+      <c r="A42" s="58"/>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="56"/>
+      <c r="A43" s="58"/>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="56"/>
+      <c r="A44" s="58"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2004,7 +2105,7 @@
       <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.16"/>
@@ -2016,33 +2117,33 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.89"/>
   </cols>
   <sheetData>
-    <row r="1" s="58" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="58" t="s">
-        <v>187</v>
-      </c>
-      <c r="B1" s="58" t="s">
-        <v>188</v>
-      </c>
-      <c r="C1" s="58" t="s">
-        <v>189</v>
-      </c>
-      <c r="D1" s="58" t="s">
-        <v>190</v>
-      </c>
-      <c r="E1" s="58" t="s">
-        <v>191</v>
-      </c>
-      <c r="F1" s="58" t="s">
-        <v>192</v>
-      </c>
-      <c r="G1" s="58" t="s">
-        <v>120</v>
-      </c>
-      <c r="H1" s="58" t="s">
-        <v>193</v>
-      </c>
-      <c r="I1" s="58" t="s">
-        <v>194</v>
+    <row r="1" s="60" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="60" t="s">
+        <v>196</v>
+      </c>
+      <c r="B1" s="60" t="s">
+        <v>197</v>
+      </c>
+      <c r="C1" s="60" t="s">
+        <v>198</v>
+      </c>
+      <c r="D1" s="60" t="s">
+        <v>199</v>
+      </c>
+      <c r="E1" s="60" t="s">
+        <v>200</v>
+      </c>
+      <c r="F1" s="60" t="s">
+        <v>201</v>
+      </c>
+      <c r="G1" s="60" t="s">
+        <v>202</v>
+      </c>
+      <c r="H1" s="60" t="s">
+        <v>203</v>
+      </c>
+      <c r="I1" s="60" t="s">
+        <v>204</v>
       </c>
       <c r="AMF1" s="0"/>
       <c r="AMG1" s="0"/>
@@ -2058,7 +2159,7 @@
         <v>78</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>195</v>
+        <v>205</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>91</v>
@@ -2070,13 +2171,13 @@
         <v>97</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>196</v>
+        <v>135</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>197</v>
+        <v>206</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2084,45 +2185,45 @@
         <v>75</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>198</v>
+        <v>207</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>199</v>
+        <v>208</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>200</v>
+        <v>209</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>87</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>201</v>
+        <v>210</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>202</v>
+        <v>211</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>203</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>205</v>
+        <v>213</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>207</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2130,18 +2231,18 @@
         <v>80</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>208</v>
+        <v>215</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>209</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
     </row>
   </sheetData>
@@ -2169,7 +2270,7 @@
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="19.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="19.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="11" width="21.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="12" width="17.71"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1018" min="5" style="13" width="11.57"/>
@@ -2447,14 +2548,14 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="11" width="17.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="20" width="16.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="11" width="19.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="11" width="19.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="11" width="19.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="11" width="18.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="21" width="18.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="21" width="17.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="11" width="19.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="11" width="19.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="11" width="17.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="11" width="24.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="12" width="16.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="12" width="16.41"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1022" min="15" style="13" width="11.57"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1023" style="1" width="11.57"/>
   </cols>
@@ -2928,7 +3029,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3048,16 +3149,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="11.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="15.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="20.57"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="4" style="1" width="11.71"/>
   </cols>
@@ -3147,18 +3248,29 @@
       </c>
       <c r="C9" s="31"/>
     </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B10" s="33" t="s">
+      <c r="B10" s="30" t="s">
         <v>117</v>
       </c>
-      <c r="C10" s="34"/>
-    </row>
-    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E20" s="1" t="s">
+      <c r="C10" s="31"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
         <v>118</v>
+      </c>
+      <c r="B11" s="33" t="s">
+        <v>119</v>
+      </c>
+      <c r="C11" s="34" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E21" s="1" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -3177,161 +3289,226 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ8"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H22" activeCellId="0" sqref="H22"/>
+      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="13" width="24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="13" width="18.67"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="6" style="13" width="11.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="8" style="1" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="13" width="18.66"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="6" style="13" width="11.57"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="10" style="1" width="11.57"/>
   </cols>
   <sheetData>
-    <row r="1" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="15" customFormat="true" ht="25.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="15" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B1" s="15" t="s">
         <v>12</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>124</v>
-      </c>
-      <c r="H1" s="15" t="s">
-        <v>125</v>
-      </c>
-      <c r="AMJ1" s="0"/>
+        <v>127</v>
+      </c>
+      <c r="H1" s="35" t="s">
+        <v>128</v>
+      </c>
+      <c r="I1" s="35" t="s">
+        <v>129</v>
+      </c>
+      <c r="J1" s="15" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>107</v>
       </c>
       <c r="B2" s="8" t="str">
-        <f aca="false">IF(C2="Absolute",Units!B6,"")</f>
-        <v/>
-      </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="29"/>
+        <f aca="false">IF(C2="Absolute",Units!B6,Units!B11)</f>
+        <v>% FM</v>
+      </c>
+      <c r="C2" s="36" t="s">
+        <v>131</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37" t="n">
+        <v>-2</v>
+      </c>
+      <c r="I2" s="37" t="n">
+        <v>4</v>
+      </c>
+      <c r="J2" s="29" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C3" s="37"/>
-      <c r="D3" s="38"/>
+        <v>133</v>
+      </c>
+      <c r="C3" s="38" t="s">
+        <v>131</v>
+      </c>
+      <c r="D3" s="39" t="s">
+        <v>134</v>
+      </c>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
       <c r="G3" s="11"/>
-      <c r="H3" s="31"/>
+      <c r="H3" s="11" t="n">
+        <v>-0.3</v>
+      </c>
+      <c r="I3" s="11" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="J3" s="31"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>63</v>
       </c>
       <c r="B4" s="8" t="str">
-        <f aca="false">IF(C4="Absolute",Units!B5,"")</f>
-        <v/>
-      </c>
-      <c r="C4" s="37"/>
-      <c r="D4" s="38"/>
+        <f aca="false">IF(C4="Absolute",Units!B5,Units!B11)</f>
+        <v>t/ha</v>
+      </c>
+      <c r="C4" s="38" t="s">
+        <v>131</v>
+      </c>
+      <c r="D4" s="39" t="s">
+        <v>132</v>
+      </c>
       <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="31"/>
+      <c r="F4" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="11" t="n">
+        <v>50</v>
+      </c>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="31" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>61</v>
       </c>
       <c r="B5" s="8" t="str">
-        <f aca="false">IF(C5="Absolute",Units!B2,"")</f>
-        <v/>
-      </c>
-      <c r="C5" s="37"/>
-      <c r="D5" s="38"/>
+        <f aca="false">IF(C5="Absolute",Units!B2,Units!B11)</f>
+        <v>Frac. input value</v>
+      </c>
+      <c r="C5" s="38" t="s">
+        <v>135</v>
+      </c>
+      <c r="D5" s="39" t="s">
+        <v>132</v>
+      </c>
       <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="31"/>
+      <c r="F5" s="11" t="n">
+        <v>-0.2</v>
+      </c>
+      <c r="G5" s="11" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="31" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>66</v>
       </c>
       <c r="B6" s="8" t="str">
-        <f aca="false">IF(C6="Absolute",Units!B8,"")</f>
-        <v/>
-      </c>
-      <c r="C6" s="37"/>
-      <c r="D6" s="38"/>
+        <f aca="false">IF(C6="Absolute",Units!B8,Units!B11)</f>
+        <v>Frac. input value</v>
+      </c>
+      <c r="C6" s="38" t="s">
+        <v>135</v>
+      </c>
+      <c r="D6" s="39" t="s">
+        <v>136</v>
+      </c>
       <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="31"/>
+      <c r="F6" s="11" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G6" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="31"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>114</v>
       </c>
       <c r="B7" s="8" t="str">
-        <f aca="false">IF(C7="Absolute",Units!B9,"")</f>
+        <f aca="false">IF(C7="Absolute",Units!B9,Units!B11)</f>
         <v>°C</v>
       </c>
-      <c r="C7" s="37" t="s">
-        <v>127</v>
-      </c>
-      <c r="D7" s="38" t="s">
-        <v>128</v>
+      <c r="C7" s="38" t="s">
+        <v>131</v>
+      </c>
+      <c r="D7" s="39" t="s">
+        <v>137</v>
       </c>
       <c r="E7" s="11" t="n">
         <v>2</v>
       </c>
       <c r="F7" s="11"/>
       <c r="G7" s="11"/>
-      <c r="H7" s="31"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="31"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>116</v>
       </c>
       <c r="B8" s="8" t="str">
-        <f aca="false">IF(C8="Absolute",Units!B10,"")</f>
+        <f aca="false">IF(C8="Absolute",Units!B10,Units!B11)</f>
         <v>m/s</v>
       </c>
-      <c r="C8" s="39" t="s">
-        <v>127</v>
-      </c>
-      <c r="D8" s="40" t="s">
-        <v>128</v>
-      </c>
-      <c r="E8" s="41" t="n">
+      <c r="C8" s="40" t="s">
+        <v>131</v>
+      </c>
+      <c r="D8" s="41" t="s">
+        <v>137</v>
+      </c>
+      <c r="E8" s="42" t="n">
         <v>0.5</v>
       </c>
-      <c r="F8" s="41"/>
-      <c r="G8" s="41"/>
-      <c r="H8" s="34"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="42"/>
+      <c r="I8" s="42"/>
+      <c r="J8" s="43"/>
     </row>
   </sheetData>
   <dataValidations count="3">
@@ -3339,7 +3516,7 @@
       <formula1>Options!$G$2:$G$3</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D1:I1 E2:I8 D9:I1008" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D1:K1 E2:K8 D9:K1008" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3355,6 +3532,7 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3373,57 +3551,57 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="25.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="13" width="23.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="13" width="17.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="42" width="12.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="42" width="30.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="13" width="17.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="44" width="12.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="44" width="30.7"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="6" style="13" width="11.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="15" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B1" s="15" t="s">
         <v>12</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="D1" s="43" t="s">
-        <v>130</v>
-      </c>
-      <c r="E1" s="43" t="s">
-        <v>131</v>
+        <v>138</v>
+      </c>
+      <c r="D1" s="45" t="s">
+        <v>139</v>
+      </c>
+      <c r="E1" s="45" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="44" t="s">
-        <v>132</v>
-      </c>
-      <c r="B2" s="44" t="s">
+      <c r="A2" s="46" t="s">
+        <v>141</v>
+      </c>
+      <c r="B2" s="46" t="s">
         <v>73</v>
       </c>
-      <c r="C2" s="45"/>
-      <c r="D2" s="42" t="n">
+      <c r="C2" s="47"/>
+      <c r="D2" s="44" t="n">
         <v>15</v>
       </c>
-      <c r="E2" s="42" t="s">
-        <v>133</v>
+      <c r="E2" s="44" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="13" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="C3" s="46"/>
-      <c r="D3" s="47" t="s">
-        <v>136</v>
-      </c>
-      <c r="E3" s="42" t="s">
-        <v>137</v>
+        <v>144</v>
+      </c>
+      <c r="C3" s="48"/>
+      <c r="D3" s="49" t="s">
+        <v>145</v>
+      </c>
+      <c r="E3" s="44" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3437,11 +3615,11 @@
       <c r="C4" s="26" t="n">
         <v>30</v>
       </c>
-      <c r="D4" s="42" t="n">
+      <c r="D4" s="44" t="n">
         <v>40</v>
       </c>
-      <c r="E4" s="48" t="s">
-        <v>138</v>
+      <c r="E4" s="50" t="s">
+        <v>147</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -3455,40 +3633,40 @@
         <v>% FM</v>
       </c>
       <c r="C5" s="26"/>
-      <c r="D5" s="42" t="n">
+      <c r="D5" s="44" t="n">
         <v>5</v>
       </c>
-      <c r="E5" s="48" t="s">
-        <v>138</v>
+      <c r="E5" s="50" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="13" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="B6" s="23"/>
       <c r="C6" s="26"/>
-      <c r="D6" s="42" t="n">
+      <c r="D6" s="44" t="n">
         <v>7</v>
       </c>
-      <c r="E6" s="48" t="s">
-        <v>138</v>
+      <c r="E6" s="50" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="13" t="s">
-        <v>139</v>
+        <v>148</v>
       </c>
       <c r="B7" s="23" t="str">
         <f aca="false">Units!B7</f>
         <v>kg/t</v>
       </c>
-      <c r="C7" s="49"/>
-      <c r="D7" s="42" t="n">
+      <c r="C7" s="51"/>
+      <c r="D7" s="44" t="n">
         <v>3</v>
       </c>
-      <c r="E7" s="48" t="s">
-        <v>138</v>
+      <c r="E7" s="50" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -3516,7 +3694,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3536,25 +3714,25 @@
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B2" s="50" t="s">
-        <v>141</v>
+        <v>149</v>
+      </c>
+      <c r="B2" s="52" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="B3" s="51" t="n">
-        <v>120178</v>
+        <v>151</v>
+      </c>
+      <c r="B3" s="53" t="n">
+        <v>123</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="B4" s="52" t="n">
+        <v>152</v>
+      </c>
+      <c r="B4" s="54" t="n">
         <v>168</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Progress in processing uncertainty output.
Put summation out of loop.
</commit_message>
<xml_diff>
--- a/inputs/inputs.xlsx
+++ b/inputs/inputs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" state="visible" r:id="rId2"/>
@@ -49,7 +49,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0">
+    <comment ref="C1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -142,7 +142,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="222">
   <si>
     <t xml:space="preserve">Combined input file for the ALFAMI R package for estimation of ammonia emission from field-applied slurry</t>
   </si>
@@ -341,6 +341,9 @@
     <t xml:space="preserve">Application event name</t>
   </si>
   <si>
+    <t xml:space="preserve">Livestock category</t>
+  </si>
+  <si>
     <t xml:space="preserve">Application year</t>
   </si>
   <si>
@@ -389,6 +392,9 @@
     <t xml:space="preserve">Cattle spring</t>
   </si>
   <si>
+    <t xml:space="preserve">Dairy cattle</t>
+  </si>
+  <si>
     <t xml:space="preserve">Trailing hose</t>
   </si>
   <si>
@@ -404,6 +410,9 @@
     <t xml:space="preserve">Pig fall</t>
   </si>
   <si>
+    <t xml:space="preserve">Swine (finishing pigs)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Open slot injection</t>
   </si>
   <si>
@@ -455,333 +464,339 @@
     <t xml:space="preserve">Type of output</t>
   </si>
   <si>
+    <t xml:space="preserve">CSV and xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Variable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slurry mass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TAN mass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Land area</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t/ha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slurry dry matter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">% FM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">% of fresh mass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TAN concentration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kg/t</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Air temperature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">°C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wind speed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m/s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Any)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frac. input value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For relative uncertainty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Input</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uncertainty type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Distribution type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Standard deviation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minimum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maximum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Centered minimum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Centered maximum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shape</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Absolute</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PERT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slurry pH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Triangular</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Relative</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uniform</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Normal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Default value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Source</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Application day of month</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assumed, middle of month</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Application time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HH:MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assumed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average from ALFAM2 database vx.x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slurry TAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parameter set</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALFAM2pars03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uncertainty seed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Emission duration (h)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">File type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Directory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weather</t>
+  </si>
+  <si>
+    <t xml:space="preserve">weather</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Output</t>
+  </si>
+  <si>
+    <t xml:space="preserve">output</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Logs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">logs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weather locations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">loc.key</t>
+  </si>
+  <si>
+    <t xml:space="preserve">loc.agg1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">loc.agg2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">loc.name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">man.key</t>
+  </si>
+  <si>
+    <t xml:space="preserve">man.source</t>
+  </si>
+  <si>
+    <t xml:space="preserve">man.dm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">man.tan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">man.ph</t>
+  </si>
+  <si>
+    <t xml:space="preserve">app.key</t>
+  </si>
+  <si>
+    <t xml:space="preserve">livestock.group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">app.year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">app.man</t>
+  </si>
+  <si>
+    <t xml:space="preserve">app.tan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">app.area</t>
+  </si>
+  <si>
+    <t xml:space="preserve">app.rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">app.mthd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">incorp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">incorp.time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wthr.year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wthr.month</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wthr.day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wthr.time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uncert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">paruncert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wthr.type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ndig</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ofile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">overwrite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">otype</t>
+  </si>
+  <si>
+    <t xml:space="preserve">parset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">seedu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">emis.dur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Application methods</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Incorporation options</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parameter sets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weather data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes/no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Output type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Relative or absolute</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mean or mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Distributions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALFAM2pars01</t>
+  </si>
+  <si>
     <t xml:space="preserve">CSV</t>
   </si>
   <si>
-    <t xml:space="preserve">Variable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Notes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Slurry mass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">t</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TAN mass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Land area</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ha</t>
-  </si>
-  <si>
-    <t xml:space="preserve">t/ha</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Slurry dry matter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">% FM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">% of fresh mass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TAN concentration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kg/t</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Air temperature</t>
-  </si>
-  <si>
-    <t xml:space="preserve">°C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wind speed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">m/s</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(Any)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Frac. input value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">For relative uncertainty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">`</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Input</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Uncertainty type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Distribution type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Standard deviation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Minimum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maximum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Centered minimum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Centered maximum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shape</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Absolute</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PERT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Slurry pH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Triangular</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Relative</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Uniform</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Normal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Default value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Source</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Application day of month</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Assumed, middle of month</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Application time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HH:MM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">09:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Assumed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Average from ALFAM2 database vx.x</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Slurry TAN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parameter set</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ALFAM2pars03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Uncertainty seed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Emission duration (h)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">File type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Directory</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Weather</t>
-  </si>
-  <si>
-    <t xml:space="preserve">weather</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Output</t>
-  </si>
-  <si>
-    <t xml:space="preserve">output</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Logs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">logs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Weather locations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">loc.key</t>
-  </si>
-  <si>
-    <t xml:space="preserve">loc.agg1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">loc.agg2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">loc.name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">man.key</t>
-  </si>
-  <si>
-    <t xml:space="preserve">man.source</t>
-  </si>
-  <si>
-    <t xml:space="preserve">man.dm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">man.tan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">man.ph</t>
-  </si>
-  <si>
-    <t xml:space="preserve">app.key</t>
-  </si>
-  <si>
-    <t xml:space="preserve">app.year</t>
-  </si>
-  <si>
-    <t xml:space="preserve">app.man</t>
-  </si>
-  <si>
-    <t xml:space="preserve">app.tan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">app.area</t>
-  </si>
-  <si>
-    <t xml:space="preserve">app.rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">app.mthd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">incorp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">incorp.time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wthr.year</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wthr.month</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wthr.day</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wthr.time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">uncert</t>
-  </si>
-  <si>
-    <t xml:space="preserve">paruncert</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wthr.type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ndig</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ofile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">overwrite</t>
-  </si>
-  <si>
-    <t xml:space="preserve">otype</t>
-  </si>
-  <si>
-    <t xml:space="preserve">parset</t>
-  </si>
-  <si>
-    <t xml:space="preserve">seedu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">emis.dur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Application methods</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Incorporation options</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parameter sets</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Weather data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes/no</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Output type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Relative or absolute</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mean or mode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Distributions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ALFAM2pars01</t>
-  </si>
-  <si>
     <t xml:space="preserve">Mean (average)</t>
   </si>
   <si>
@@ -807,9 +822,6 @@
   </si>
   <si>
     <t xml:space="preserve">xlsx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CSV and xlsx</t>
   </si>
   <si>
     <t xml:space="preserve">Closed slot injection</t>
@@ -1597,34 +1609,34 @@
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="28" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="30" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="B3" s="31" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="33" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="B4" s="34" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -1643,38 +1655,40 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O44"/>
+  <dimension ref="A1:AMJ44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="55" width="26.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="11" width="19.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="11" width="11.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="11" width="17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="11" width="15.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="11" width="15.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="11" width="15.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="11" width="18.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="11" width="13.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="11" width="18.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="11" width="12.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="11" width="17.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="11" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="11" width="15.71"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="16" style="11" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="55" width="19.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="11" width="19.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="11" width="11.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="11" width="17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="11" width="15.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="11" width="15.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="11" width="15.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="11" width="18.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="11" width="13.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="11" width="18.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="11" width="12.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="11" width="17.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="11" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="11" width="15.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="17" style="11" width="11.57"/>
   </cols>
   <sheetData>
     <row r="1" s="57" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="56" t="s">
-        <v>161</v>
-      </c>
-      <c r="B1" s="11"/>
+        <v>164</v>
+      </c>
+      <c r="B1" s="56"/>
       <c r="C1" s="11"/>
       <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="58" t="str">
@@ -1698,20 +1712,26 @@
       <c r="G2" s="57"/>
       <c r="H2" s="57"/>
       <c r="I2" s="57"/>
+      <c r="AMJ2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="55" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>165</v>
-      </c>
+        <v>168</v>
+      </c>
+      <c r="AMJ3" s="0"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="11"/>
+      <c r="AMJ4" s="0"/>
     </row>
     <row r="5" s="57" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="56" t="s">
@@ -1720,6 +1740,7 @@
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
+      <c r="AMJ5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="58" t="str">
@@ -1742,139 +1763,150 @@
         <f aca="false">'Slurry composition'!E1</f>
         <v>pH</v>
       </c>
+      <c r="AMJ6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="55" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>170</v>
-      </c>
+        <v>173</v>
+      </c>
+      <c r="AMJ7" s="0"/>
     </row>
     <row r="9" s="57" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="11"/>
+      <c r="B9" s="56"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
-    </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E9" s="11"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="58" t="str">
         <f aca="false">Application!A1</f>
         <v>Application event name</v>
       </c>
       <c r="B10" s="57" t="str">
         <f aca="false">Application!B1</f>
-        <v>Location key</v>
+        <v>Livestock category</v>
       </c>
       <c r="C10" s="57" t="str">
         <f aca="false">Application!C1</f>
-        <v>Application year</v>
+        <v>Location key</v>
       </c>
       <c r="D10" s="57" t="str">
         <f aca="false">Application!D1</f>
-        <v>Slurry key</v>
+        <v>Application year</v>
       </c>
       <c r="E10" s="57" t="str">
         <f aca="false">Application!E1</f>
-        <v>Slurry application</v>
+        <v>Slurry key</v>
       </c>
       <c r="F10" s="57" t="str">
         <f aca="false">Application!F1</f>
-        <v>TAN application</v>
+        <v>Slurry application</v>
       </c>
       <c r="G10" s="57" t="str">
         <f aca="false">Application!G1</f>
-        <v>Application area</v>
+        <v>TAN application</v>
       </c>
       <c r="H10" s="57" t="str">
         <f aca="false">Application!H1</f>
-        <v>Application rate</v>
+        <v>Application area</v>
       </c>
       <c r="I10" s="57" t="str">
         <f aca="false">Application!I1</f>
-        <v>Application method</v>
+        <v>Application rate</v>
       </c>
       <c r="J10" s="57" t="str">
         <f aca="false">Application!J1</f>
-        <v>Incorporation</v>
+        <v>Application method</v>
       </c>
       <c r="K10" s="57" t="str">
         <f aca="false">Application!K1</f>
-        <v>Incorporation delay</v>
+        <v>Incorporation</v>
       </c>
       <c r="L10" s="57" t="str">
         <f aca="false">Application!L1</f>
-        <v>Weather year</v>
+        <v>Incorporation delay</v>
       </c>
       <c r="M10" s="57" t="str">
         <f aca="false">Application!M1</f>
-        <v>Application month</v>
+        <v>Weather year</v>
       </c>
       <c r="N10" s="57" t="str">
         <f aca="false">Application!N1</f>
+        <v>Application month</v>
+      </c>
+      <c r="O10" s="57" t="str">
+        <f aca="false">Application!O1</f>
         <v>Application day</v>
       </c>
-      <c r="O10" s="57"/>
+      <c r="P10" s="57"/>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="55" t="s">
-        <v>171</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>162</v>
+        <v>174</v>
+      </c>
+      <c r="B11" s="55" t="s">
+        <v>175</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="H11" s="11" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="I11" s="11" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="J11" s="11" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="K11" s="11" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="L11" s="11" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="M11" s="11" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="N11" s="11" t="s">
-        <v>182</v>
+        <v>185</v>
+      </c>
+      <c r="O11" s="11" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="56" t="s">
         <v>16</v>
       </c>
+      <c r="B13" s="56"/>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="58" t="str">
@@ -1882,10 +1914,11 @@
         <v>Application day of month</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="C14" s="57"/>
       <c r="D14" s="57"/>
+      <c r="AMJ14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="59" t="str">
@@ -1893,8 +1926,9 @@
         <v>Application time</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>183</v>
-      </c>
+        <v>187</v>
+      </c>
+      <c r="AMJ15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="58" t="str">
@@ -1902,8 +1936,9 @@
         <v>Application rate</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>176</v>
-      </c>
+        <v>180</v>
+      </c>
+      <c r="AMJ16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="58" t="str">
@@ -1911,8 +1946,9 @@
         <v>Slurry dry matter</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>168</v>
-      </c>
+        <v>171</v>
+      </c>
+      <c r="AMJ17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="58" t="str">
@@ -1920,8 +1956,9 @@
         <v>Slurry pH</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>170</v>
-      </c>
+        <v>173</v>
+      </c>
+      <c r="AMJ18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="58" t="str">
@@ -1929,16 +1966,19 @@
         <v>Slurry TAN</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>172</v>
+      </c>
+      <c r="AMJ19" s="0"/>
+    </row>
+    <row r="20" s="11" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="58"/>
-    </row>
-    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AMJ20" s="0"/>
+    </row>
+    <row r="21" s="11" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="56" t="s">
         <v>10</v>
       </c>
+      <c r="AMJ21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="58" t="str">
@@ -1946,8 +1986,9 @@
         <v>Include input uncertainty?</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>184</v>
-      </c>
+        <v>188</v>
+      </c>
+      <c r="AMJ22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="58" t="str">
@@ -1955,8 +1996,9 @@
         <v>Include par uncertainty?</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>185</v>
-      </c>
+        <v>189</v>
+      </c>
+      <c r="AMJ23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="58" t="str">
@@ -1964,8 +2006,9 @@
         <v>Uncertainty iterations</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>186</v>
-      </c>
+        <v>190</v>
+      </c>
+      <c r="AMJ24" s="0"/>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="58" t="str">
@@ -1973,8 +2016,9 @@
         <v>Confidence level</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>187</v>
-      </c>
+        <v>191</v>
+      </c>
+      <c r="AMJ25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="58" t="str">
@@ -1982,8 +2026,9 @@
         <v>Weather resolution</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>188</v>
-      </c>
+        <v>192</v>
+      </c>
+      <c r="AMJ26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="58" t="str">
@@ -1991,8 +2036,9 @@
         <v>Output digits</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>189</v>
-      </c>
+        <v>193</v>
+      </c>
+      <c r="AMJ27" s="0"/>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="58" t="str">
@@ -2000,8 +2046,9 @@
         <v>Output file name</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>190</v>
-      </c>
+        <v>194</v>
+      </c>
+      <c r="AMJ28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="58" t="str">
@@ -2009,8 +2056,9 @@
         <v>Overwrite output?</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>191</v>
-      </c>
+        <v>195</v>
+      </c>
+      <c r="AMJ29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="58" t="str">
@@ -2018,16 +2066,19 @@
         <v>Type of output</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>196</v>
+      </c>
+      <c r="AMJ30" s="0"/>
+    </row>
+    <row r="31" s="11" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="58"/>
-    </row>
-    <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AMJ31" s="0"/>
+    </row>
+    <row r="32" s="11" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="56" t="s">
         <v>18</v>
       </c>
+      <c r="AMJ32" s="0"/>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="58" t="str">
@@ -2035,8 +2086,9 @@
         <v>Parameter set</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>193</v>
-      </c>
+        <v>197</v>
+      </c>
+      <c r="AMJ33" s="0"/>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="58" t="str">
@@ -2044,8 +2096,9 @@
         <v>Uncertainty seed</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>194</v>
-      </c>
+        <v>198</v>
+      </c>
+      <c r="AMJ34" s="0"/>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="58" t="str">
@@ -2053,35 +2106,45 @@
         <v>Emission duration (h)</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>195</v>
-      </c>
+        <v>199</v>
+      </c>
+      <c r="AMJ35" s="0"/>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="58"/>
+      <c r="B36" s="58"/>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="58"/>
+      <c r="B37" s="58"/>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="58"/>
+      <c r="B38" s="58"/>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="58"/>
+      <c r="B39" s="58"/>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="58"/>
+      <c r="B40" s="58"/>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="58"/>
+      <c r="B41" s="58"/>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="58"/>
+      <c r="B42" s="58"/>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="58"/>
+      <c r="B43" s="58"/>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="58"/>
+      <c r="B44" s="58"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2119,31 +2182,31 @@
   <sheetData>
     <row r="1" s="60" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="60" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="B1" s="60" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="C1" s="60" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="D1" s="60" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="E1" s="60" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="F1" s="60" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="G1" s="60" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="H1" s="60" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="I1" s="60" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="AMF1" s="0"/>
       <c r="AMG1" s="0"/>
@@ -2153,96 +2216,96 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>97</v>
+        <v>210</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>215</v>
+        <v>100</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
     </row>
   </sheetData>
@@ -2538,43 +2601,44 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="36.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="20" width="17.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="11" width="17.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="20" width="16.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="11" width="19.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="11" width="19.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="11" width="18.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="21" width="18.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="21" width="17.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="11" width="19.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="11" width="17.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="11" width="24.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="12" width="16.41"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1022" min="15" style="13" width="11.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1023" style="1" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="18.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="20" width="17.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="11" width="17.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="20" width="16.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="11" width="19.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="11" width="19.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="11" width="18.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="21" width="18.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="21" width="17.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="11" width="19.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="11" width="17.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="11" width="24.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="12" width="16.41"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="16" style="13" width="11.57"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1024" style="1" width="11.57"/>
   </cols>
   <sheetData>
-    <row r="1" s="15" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" s="14" t="s">
         <v>45</v>
-      </c>
-      <c r="E1" s="15" t="s">
-        <v>60</v>
       </c>
       <c r="F1" s="15" t="s">
         <v>61</v>
@@ -2585,13 +2649,13 @@
       <c r="H1" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="I1" s="22" t="s">
+      <c r="I1" s="15" t="s">
         <v>64</v>
       </c>
       <c r="J1" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="K1" s="15" t="s">
+      <c r="K1" s="22" t="s">
         <v>66</v>
       </c>
       <c r="L1" s="15" t="s">
@@ -2603,409 +2667,446 @@
       <c r="N1" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="AMI1" s="1"/>
+      <c r="O1" s="15" t="s">
+        <v>70</v>
+      </c>
       <c r="AMJ1" s="1"/>
     </row>
-    <row r="2" s="15" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="C2" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="D2" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="E2" s="23" t="str">
-        <f aca="false">Units!B2</f>
-        <v>t</v>
+      <c r="C2" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>71</v>
       </c>
       <c r="F2" s="23" t="str">
         <f aca="false">Units!B2</f>
         <v>t</v>
       </c>
       <c r="G2" s="23" t="str">
+        <f aca="false">Units!B2</f>
+        <v>t</v>
+      </c>
+      <c r="H2" s="23" t="str">
         <f aca="false">Units!B4</f>
         <v>ha</v>
       </c>
-      <c r="H2" s="23" t="str">
+      <c r="I2" s="23" t="str">
         <f aca="false">Units!B5</f>
         <v>t/ha</v>
       </c>
-      <c r="I2" s="22" t="s">
-        <v>70</v>
-      </c>
       <c r="J2" s="22" t="s">
-        <v>70</v>
-      </c>
-      <c r="K2" s="15" t="str">
+        <v>71</v>
+      </c>
+      <c r="K2" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="L2" s="15" t="str">
         <f aca="false">Units!B8</f>
         <v>hr</v>
       </c>
-      <c r="L2" s="15" t="s">
-        <v>71</v>
-      </c>
       <c r="M2" s="15" t="s">
         <v>72</v>
       </c>
       <c r="N2" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="AMI2" s="1"/>
+      <c r="O2" s="15" t="s">
+        <v>74</v>
+      </c>
       <c r="AMJ2" s="1"/>
     </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="B3" s="20" t="n">
+        <v>75</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" s="20" t="n">
         <v>1000</v>
       </c>
-      <c r="C3" s="11" t="n">
+      <c r="D3" s="11" t="n">
         <v>2019</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="E3" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="F3" s="11" t="n">
+      <c r="G3" s="11" t="n">
         <v>350</v>
       </c>
-      <c r="I3" s="21" t="s">
+      <c r="J3" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="M3" s="11" t="n">
+        <v>2019</v>
+      </c>
+      <c r="N3" s="11" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" s="20" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D4" s="11" t="n">
+        <v>2019</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="G4" s="11" t="n">
+        <v>720</v>
+      </c>
+      <c r="J4" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="K4" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="L4" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="M4" s="11" t="n">
+        <v>2019</v>
+      </c>
+      <c r="N4" s="11" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" s="20" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D5" s="11" t="n">
+        <v>2019</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="G5" s="11" t="n">
+        <v>1240</v>
+      </c>
+      <c r="J5" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="M5" s="11" t="n">
+        <v>2019</v>
+      </c>
+      <c r="N5" s="11" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" s="20" t="n">
+        <v>1001</v>
+      </c>
+      <c r="D6" s="11" t="n">
+        <v>2019</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="G6" s="11" t="n">
+        <v>3520</v>
+      </c>
+      <c r="J6" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="M6" s="11" t="n">
+        <v>2019</v>
+      </c>
+      <c r="N6" s="11" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="L3" s="11" t="n">
+      <c r="B7" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" s="20" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D7" s="11" t="n">
+        <v>2020</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="G7" s="11" t="n">
+        <v>420</v>
+      </c>
+      <c r="J7" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="M7" s="11" t="n">
+        <v>2020</v>
+      </c>
+      <c r="N7" s="11" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="C8" s="20" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D8" s="11" t="n">
+        <v>2020</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="G8" s="11" t="n">
+        <v>1000</v>
+      </c>
+      <c r="J8" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="K8" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="L8" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="M8" s="11" t="n">
+        <v>2020</v>
+      </c>
+      <c r="N8" s="11" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="C9" s="20" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D9" s="11" t="n">
+        <v>2020</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="G9" s="11" t="n">
+        <v>1190</v>
+      </c>
+      <c r="J9" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="M9" s="11" t="n">
+        <v>2020</v>
+      </c>
+      <c r="N9" s="11" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10" s="20" t="n">
+        <v>1001</v>
+      </c>
+      <c r="D10" s="11" t="n">
+        <v>2020</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="G10" s="11" t="n">
+        <v>3300</v>
+      </c>
+      <c r="J10" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="M10" s="11" t="n">
+        <v>2020</v>
+      </c>
+      <c r="N10" s="11" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="C11" s="20" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D11" s="11" t="n">
+        <v>2021</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="G11" s="11" t="n">
+        <v>350</v>
+      </c>
+      <c r="J11" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="M11" s="11" t="n">
         <v>2019</v>
       </c>
-      <c r="M3" s="11" t="n">
+      <c r="N11" s="11" t="n">
         <v>4</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="11" t="s">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B12" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="B4" s="20" t="n">
+      <c r="C12" s="20" t="n">
         <v>1000</v>
       </c>
-      <c r="C4" s="11" t="n">
+      <c r="D12" s="11" t="n">
+        <v>2021</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="G12" s="11" t="n">
+        <v>720</v>
+      </c>
+      <c r="J12" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="K12" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="L12" s="11" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="M12" s="11" t="n">
         <v>2019</v>
       </c>
-      <c r="D4" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="F4" s="11" t="n">
-        <v>720</v>
-      </c>
-      <c r="I4" s="21" t="s">
+      <c r="N12" s="11" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="C13" s="20" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D13" s="11" t="n">
+        <v>2021</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="G13" s="11" t="n">
+        <v>1240</v>
+      </c>
+      <c r="J13" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="M13" s="11" t="n">
+        <v>2019</v>
+      </c>
+      <c r="N13" s="11" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="C14" s="20" t="n">
+        <v>1001</v>
+      </c>
+      <c r="D14" s="11" t="n">
+        <v>2021</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="G14" s="11" t="n">
+        <v>3520</v>
+      </c>
+      <c r="J14" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="J4" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="K4" s="11" t="n">
-        <v>4</v>
-      </c>
-      <c r="L4" s="11" t="n">
+      <c r="M14" s="11" t="n">
         <v>2019</v>
       </c>
-      <c r="M4" s="11" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="B5" s="20" t="n">
-        <v>1000</v>
-      </c>
-      <c r="C5" s="11" t="n">
-        <v>2019</v>
-      </c>
-      <c r="D5" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="F5" s="11" t="n">
-        <v>1240</v>
-      </c>
-      <c r="I5" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="L5" s="11" t="n">
-        <v>2019</v>
-      </c>
-      <c r="M5" s="11" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="B6" s="20" t="n">
-        <v>1001</v>
-      </c>
-      <c r="C6" s="11" t="n">
-        <v>2019</v>
-      </c>
-      <c r="D6" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="F6" s="11" t="n">
-        <v>3520</v>
-      </c>
-      <c r="I6" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="L6" s="11" t="n">
-        <v>2019</v>
-      </c>
-      <c r="M6" s="11" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="B7" s="20" t="n">
-        <v>1000</v>
-      </c>
-      <c r="C7" s="11" t="n">
-        <v>2020</v>
-      </c>
-      <c r="D7" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="F7" s="11" t="n">
-        <v>420</v>
-      </c>
-      <c r="I7" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="L7" s="11" t="n">
-        <v>2020</v>
-      </c>
-      <c r="M7" s="11" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="B8" s="20" t="n">
-        <v>1000</v>
-      </c>
-      <c r="C8" s="11" t="n">
-        <v>2020</v>
-      </c>
-      <c r="D8" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="F8" s="11" t="n">
-        <v>1000</v>
-      </c>
-      <c r="I8" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="J8" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="K8" s="11" t="n">
-        <v>2</v>
-      </c>
-      <c r="L8" s="11" t="n">
-        <v>2020</v>
-      </c>
-      <c r="M8" s="11" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="B9" s="20" t="n">
-        <v>1000</v>
-      </c>
-      <c r="C9" s="11" t="n">
-        <v>2020</v>
-      </c>
-      <c r="D9" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="F9" s="11" t="n">
-        <v>1190</v>
-      </c>
-      <c r="I9" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="L9" s="11" t="n">
-        <v>2020</v>
-      </c>
-      <c r="M9" s="11" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="B10" s="20" t="n">
-        <v>1001</v>
-      </c>
-      <c r="C10" s="11" t="n">
-        <v>2020</v>
-      </c>
-      <c r="D10" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="F10" s="11" t="n">
-        <v>3300</v>
-      </c>
-      <c r="I10" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="L10" s="11" t="n">
-        <v>2020</v>
-      </c>
-      <c r="M10" s="11" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="B11" s="20" t="n">
-        <v>1000</v>
-      </c>
-      <c r="C11" s="11" t="n">
-        <v>2021</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="F11" s="11" t="n">
-        <v>350</v>
-      </c>
-      <c r="I11" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="L11" s="11" t="n">
-        <v>2019</v>
-      </c>
-      <c r="M11" s="11" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="B12" s="20" t="n">
-        <v>1000</v>
-      </c>
-      <c r="C12" s="11" t="n">
-        <v>2021</v>
-      </c>
-      <c r="D12" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="F12" s="11" t="n">
-        <v>720</v>
-      </c>
-      <c r="I12" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="J12" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="K12" s="11" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="L12" s="11" t="n">
-        <v>2019</v>
-      </c>
-      <c r="M12" s="11" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="B13" s="20" t="n">
-        <v>1000</v>
-      </c>
-      <c r="C13" s="11" t="n">
-        <v>2021</v>
-      </c>
-      <c r="D13" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="F13" s="11" t="n">
-        <v>1240</v>
-      </c>
-      <c r="I13" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="L13" s="11" t="n">
-        <v>2019</v>
-      </c>
-      <c r="M13" s="11" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="B14" s="20" t="n">
-        <v>1001</v>
-      </c>
-      <c r="C14" s="11" t="n">
-        <v>2021</v>
-      </c>
-      <c r="D14" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="F14" s="11" t="n">
-        <v>3520</v>
-      </c>
-      <c r="I14" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="L14" s="11" t="n">
-        <v>2019</v>
-      </c>
-      <c r="M14" s="11" t="n">
+      <c r="N14" s="11" t="n">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="5">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E1:E1002" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F1:F1002" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D3:D34" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E3:E34" type="list">
       <formula1>'Slurry composition'!$A$3:$A$20</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B3:B34" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C3:C34" type="list">
       <formula1>Locations!$A$2:$A$18</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I3:I100" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J3:J100" type="list">
       <formula1>Options!$A$2:$A$7</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J3:J35" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K3:K35" type="list">
       <formula1>Options!$B$2:$B$5</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3028,8 +3129,8 @@
   </sheetPr>
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J20" activeCellId="0" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3041,39 +3142,39 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B4" s="26" t="n">
-        <v>100</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B5" s="26" t="n">
         <v>0.75</v>
@@ -3081,15 +3182,15 @@
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B7" s="26" t="n">
         <v>4</v>
@@ -3097,26 +3198,26 @@
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B10" s="27" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -3165,112 +3266,112 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="C2" s="29"/>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="C3" s="31"/>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C4" s="31"/>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="C5" s="31"/>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="C6" s="31" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="B7" s="30" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="C7" s="31"/>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B8" s="30" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C8" s="31"/>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B9" s="32" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="C9" s="31"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B10" s="30" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="C10" s="31"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B11" s="33" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="C11" s="34" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E21" s="1" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -3307,49 +3408,49 @@
   <sheetData>
     <row r="1" s="15" customFormat="true" ht="25.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="15" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B1" s="15" t="s">
         <v>12</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="H1" s="35" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="I1" s="35" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="J1" s="15" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B2" s="8" t="str">
         <f aca="false">IF(C2="Absolute",Units!B6,Units!B11)</f>
         <v>% FM</v>
       </c>
       <c r="C2" s="36" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="E2" s="37"/>
       <c r="F2" s="37"/>
@@ -3366,13 +3467,13 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="C3" s="38" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="D3" s="39" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
@@ -3387,17 +3488,17 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B4" s="8" t="str">
         <f aca="false">IF(C4="Absolute",Units!B5,Units!B11)</f>
         <v>t/ha</v>
       </c>
       <c r="C4" s="38" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="D4" s="39" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="E4" s="11"/>
       <c r="F4" s="11" t="n">
@@ -3414,17 +3515,17 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B5" s="8" t="str">
         <f aca="false">IF(C5="Absolute",Units!B2,Units!B11)</f>
         <v>Frac. input value</v>
       </c>
       <c r="C5" s="38" t="s">
+        <v>138</v>
+      </c>
+      <c r="D5" s="39" t="s">
         <v>135</v>
-      </c>
-      <c r="D5" s="39" t="s">
-        <v>132</v>
       </c>
       <c r="E5" s="11"/>
       <c r="F5" s="11" t="n">
@@ -3441,17 +3542,17 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B6" s="8" t="str">
         <f aca="false">IF(C6="Absolute",Units!B8,Units!B11)</f>
         <v>Frac. input value</v>
       </c>
       <c r="C6" s="38" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D6" s="39" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="E6" s="11"/>
       <c r="F6" s="11" t="n">
@@ -3466,17 +3567,17 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B7" s="8" t="str">
         <f aca="false">IF(C7="Absolute",Units!B9,Units!B11)</f>
         <v>°C</v>
       </c>
       <c r="C7" s="38" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="D7" s="39" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="E7" s="11" t="n">
         <v>2</v>
@@ -3489,17 +3590,17 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B8" s="8" t="str">
         <f aca="false">IF(C8="Absolute",Units!B10,Units!B11)</f>
         <v>m/s</v>
       </c>
       <c r="C8" s="40" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="D8" s="41" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="E8" s="42" t="n">
         <v>0.5</v>
@@ -3559,54 +3660,54 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="15" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B1" s="15" t="s">
         <v>12</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D1" s="45" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="E1" s="45" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="46" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C2" s="47"/>
       <c r="D2" s="44" t="n">
         <v>15</v>
       </c>
       <c r="E2" s="44" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="13" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="C3" s="48"/>
       <c r="D3" s="49" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="E3" s="44" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="13" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B4" s="23" t="str">
         <f aca="false">Units!B5</f>
@@ -3619,14 +3720,14 @@
         <v>40</v>
       </c>
       <c r="E4" s="50" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="13" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B5" s="23" t="str">
         <f aca="false">Units!B6</f>
@@ -3637,12 +3738,12 @@
         <v>5</v>
       </c>
       <c r="E5" s="50" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="13" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B6" s="23"/>
       <c r="C6" s="26"/>
@@ -3650,12 +3751,12 @@
         <v>7</v>
       </c>
       <c r="E6" s="50" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="13" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="B7" s="23" t="str">
         <f aca="false">Units!B7</f>
@@ -3666,7 +3767,7 @@
         <v>3</v>
       </c>
       <c r="E7" s="50" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -3706,23 +3807,23 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="B2" s="52" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="B3" s="53" t="n">
         <v>123</v>
@@ -3730,7 +3831,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="B4" s="54" t="n">
         <v>168</v>

</xml_diff>

<commit_message>
Finish uncert output processing, change export
</commit_message>
<xml_diff>
--- a/inputs/inputs.xlsx
+++ b/inputs/inputs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="10"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" state="visible" r:id="rId2"/>
@@ -1657,8 +1657,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P14" activeCellId="0" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2327,7 +2327,7 @@
   <dimension ref="A1:AMJ6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3129,7 +3129,7 @@
   </sheetPr>
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J20" activeCellId="0" sqref="J20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Small tweaks for ALFAM2 v4.1.5
</commit_message>
<xml_diff>
--- a/inputs/inputs.xlsx
+++ b/inputs/inputs.xlsx
@@ -19,7 +19,7 @@
     <sheet name="Reproducibility" sheetId="9" state="visible" r:id="rId10"/>
     <sheet name="Directories" sheetId="10" state="visible" r:id="rId11"/>
     <sheet name="Names" sheetId="11" state="hidden" r:id="rId12"/>
-    <sheet name="Options" sheetId="12" state="hidden" r:id="rId13"/>
+    <sheet name="Options" sheetId="12" state="visible" r:id="rId13"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -620,7 +620,7 @@
     <t xml:space="preserve">Parameter set</t>
   </si>
   <si>
-    <t xml:space="preserve">ALFAM2pars02</t>
+    <t xml:space="preserve">alfam2pars03</t>
   </si>
   <si>
     <t xml:space="preserve">Uncertainty seed</t>
@@ -788,7 +788,7 @@
     <t xml:space="preserve">Distributions</t>
   </si>
   <si>
-    <t xml:space="preserve">ALFAM2pars01</t>
+    <t xml:space="preserve">alfam2pars01</t>
   </si>
   <si>
     <t xml:space="preserve">CSV</t>
@@ -800,6 +800,9 @@
     <t xml:space="preserve">Deep</t>
   </si>
   <si>
+    <t xml:space="preserve">alfam2pars02</t>
+  </si>
+  <si>
     <t xml:space="preserve">Daily</t>
   </si>
   <si>
@@ -813,9 +816,6 @@
   </si>
   <si>
     <t xml:space="preserve">Trailing shoe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ALFAM2pars03</t>
   </si>
   <si>
     <t xml:space="preserve">Sub-daily</t>
@@ -2165,10 +2165,10 @@
   <dimension ref="A1:AMJ6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.16"/>
@@ -2251,22 +2251,22 @@
         <v>211</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>152</v>
+        <v>212</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G3" s="0" t="s">
         <v>133</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="I3" s="0" t="s">
         <v>138</v>
@@ -2274,10 +2274,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>217</v>
+        <v>152</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>218</v>

</xml_diff>